<commit_message>
Updated Save_transcripts file for Call Transcripts
</commit_message>
<xml_diff>
--- a/CallTranscripts_Script/CallTranscript_DownloadTemplate.xlsx
+++ b/CallTranscripts_Script/CallTranscript_DownloadTemplate.xlsx
@@ -1,47 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshitachawdhary/Desktop/DA_Davidson/Capstone_NLP_DIWD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FC07C9-5D28-4F3B-BE9D-BE8B5FB2467B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Ticker</t>
-  </si>
-  <si>
-    <t>Quarter</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>q1</t>
   </si>
   <si>
     <t>MSFT</t>
@@ -80,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,85 +386,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>